<commit_message>
Fix Agent Inference + Data Truncation
</commit_message>
<xml_diff>
--- a/data/examples/cnn_dm_template.xlsx
+++ b/data/examples/cnn_dm_template.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Daniel Radcliffe, the star of the Harry Potter films, turns 18 and gains access to a £20 million ($41.1 million) fortune. Despite his newfound wealth, Radcliffe plans to avoid extravagant spending and maintain a modest lifestyle, preferring to buy books, CDs, and DVDs. He has no intention of indulging in fast cars, alcohol, or celebrity parties. Radcliffe's earnings from the first five Harry Potter films were held in a trust fund until his 18th birthday. He remains grounded despite his fame and fortune, aiming to avoid the pitfalls often associated with child stars. Radcliffe's latest film, "Harry Potter and the Order of the Phoenix," is a box office success, and he will continue to play Harry Potter in the final two films. Beyond Harry Potter, he has roles in the TV movie "My Boy Jack" and the Australian film "December Boys," and he recently made his stage debut in "Equus." As he becomes a legal adult, Radcliffe anticipates increased media scrutiny.</t>
+          <t>- Daniel Radcliffe gains access to a £20 million fortune as he turns 18 . - He plans to avoid extravagant spending and maintain a modest lifestyle . - Radcliffe continues to act in Harry Potter films and other projects . - He anticipates increased media scrutiny now that he</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -477,7 +477,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The article, part of CNN's Behind the Scenes series, explores the conditions on the "forgotten floor" of the Miami-Dade pretrial detention facility, where inmates with severe mental illnesses are held. These inmates often face avoidable felony charges, typically resulting from confrontations with police. Judge Steven Leifman, an advocate for the mentally ill, highlights the inadequate treatment these inmates receive in jail, which exacerbates their conditions. Historically, mentally ill individuals were either jailed or placed in mental hospitals, many of which were shut down, leading to increased homelessness. Leifman is working to change this system, with a new mental health facility set to open in 2008, aiming to provide long-term treatment rather than punishment. This initiative is expected to benefit patients, relieve families, and save state funds by reducing the cycle of re-incarceration.</t>
+          <t>- The ninth floor of Miami-Dade pretrial detention facility houses severely mentally ill inmates . - Judge Steven Leifman advocates for better treatment and justice for mentally ill prisoners . - Many mentally ill inmates cycle between jail and mental hospitals without proper treatment . - Starting in 2008 , a new mental health facility aims to provide long-term treatment</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -497,7 +497,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The article describes the harrowing experiences of survivors from the Minneapolis bridge collapse over the Mississippi River. Gary Babineau, one of the survivors, recounted his 30-35 foot free fall and subsequent efforts to rescue children from a nearby school bus. Emergency room physician Dr. John Hink rushed to the scene and helped organize the rescue efforts, which involved volunteers, EMTs, and officials managing to get 55 people into ambulances within two hours. Melissa Hughes, another survivor, described the surreal experience of her car being landed on by a pickup truck but escaping unhurt. Bernie Toivonen shared his experience of his vehicle ending up at a 45-degree angle, thinking he was going to die but ultimately surviving. The rescue efforts were described as controlled and organized despite the chaos of the collapse.</t>
+          <t>- The Minneapolis bridge collapsed , causing a 30-35 foot free fall for vehicles , with cars in the water and on fire . - Survivors , including Gary Babineau , helped rescue children from a school bus . - Emergency responders and volunteers managed to get 55 people into ambulances within two hours . - Witnesses described the scene</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>